<commit_message>
Changed forecasted energy file
</commit_message>
<xml_diff>
--- a/forecasted_energy.xlsx
+++ b/forecasted_energy.xlsx
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>67215.43566852933</v>
+        <v>78150.1224852913</v>
       </c>
     </row>
     <row r="3">
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>63724.96605913646</v>
+        <v>73931.51120751112</v>
       </c>
     </row>
     <row r="4">
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>61062.15186725625</v>
+        <v>70665.639883871</v>
       </c>
     </row>
     <row r="5">
@@ -462,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>58690.39048434388</v>
+        <v>68221.08144896063</v>
       </c>
     </row>
     <row r="6">
@@ -470,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>57953.41081697737</v>
+        <v>67442.62655372635</v>
       </c>
     </row>
     <row r="7">
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>58513.92399294129</v>
+        <v>67697.40905076484</v>
       </c>
     </row>
     <row r="8">
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>58560.18761346512</v>
+        <v>66805.99719848631</v>
       </c>
     </row>
     <row r="9">
@@ -494,7 +494,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>61749.84626794878</v>
+        <v>73518.8360027173</v>
       </c>
     </row>
     <row r="10">
@@ -502,7 +502,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>70574.08841398767</v>
+        <v>90665.86311579018</v>
       </c>
     </row>
     <row r="11">
@@ -510,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>78215.70537354975</v>
+        <v>99986.44599549515</v>
       </c>
     </row>
     <row r="12">
@@ -518,7 +518,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>82056.68372650631</v>
+        <v>104010.8232173354</v>
       </c>
     </row>
     <row r="13">
@@ -526,7 +526,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>83494.33321479897</v>
+        <v>106016.5690550003</v>
       </c>
     </row>
     <row r="14">
@@ -534,7 +534,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>83824.15966913324</v>
+        <v>107320.0925482591</v>
       </c>
     </row>
     <row r="15">
@@ -542,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>87684.05903897769</v>
+        <v>111547.1563226645</v>
       </c>
     </row>
     <row r="16">
@@ -550,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>88802.73964341768</v>
+        <v>112002.2930044165</v>
       </c>
     </row>
     <row r="17">
@@ -558,7 +558,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>86996.52656865345</v>
+        <v>109747.5369375676</v>
       </c>
     </row>
     <row r="18">
@@ -566,7 +566,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>84935.95057665437</v>
+        <v>103869.0857919438</v>
       </c>
     </row>
     <row r="19">
@@ -574,7 +574,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>81144.72874415584</v>
+        <v>96041.01666867564</v>
       </c>
     </row>
     <row r="20">
@@ -582,7 +582,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>83246.884137196</v>
+        <v>95816.15130808466</v>
       </c>
     </row>
     <row r="21">
@@ -590,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>80548.97919203494</v>
+        <v>92433.58920697204</v>
       </c>
     </row>
     <row r="22">
@@ -598,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>78069.16904515574</v>
+        <v>90165.2556892329</v>
       </c>
     </row>
     <row r="23">
@@ -606,7 +606,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>76168.53320712211</v>
+        <v>89664.82647591364</v>
       </c>
     </row>
     <row r="24">
@@ -614,7 +614,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>72298.03743205291</v>
+        <v>86158.80010198322</v>
       </c>
     </row>
     <row r="25">
@@ -622,7 +622,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>67378.63761467961</v>
+        <v>81709.70824788923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>